<commit_message>
Updated variations of questions to improve recognition accuracy
Changes made to update_from_excel.py to ensure all questions were extracted.
</commit_message>
<xml_diff>
--- a/Q&A.xlsx
+++ b/Q&A.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447B56E7-523A-4435-89A6-40E86EEF57CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7007DF92-9927-4124-A28E-F4E5DD0A58C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>Thủ tục BHYT</t>
   </si>
   <si>
-    <t>Tôi muốn hỏi về Bảo hiểm Y tế tại Bệnh viện?</t>
-  </si>
-  <si>
     <t>Xin gửi bạn tham khảo thông tin hướng dẫn thủ tục khám bệnh, chữa bệnh BHYT tại Bệnh viện Đại học Y Dược TPHCM nhé: http://bvdaihoc.com.vn/Home/ViewDetail/5128#maincontent
 Thân chào bạn.</t>
   </si>
@@ -63,9 +60,6 @@
     <t>BHYT trái tuyến</t>
   </si>
   <si>
-    <t>Bệnh viện có nhận bảo hiểm trái tuyến không?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Bạn cần có giấy chuyển tuyến để hưởng BHYT tại Bệnh viện. Bạn vui lòng liên hệ Phòng Bảo hiểm Y tế theo số điện thoại: (028) 3952 5372 (giờ hành chính) để được hướng dẫn cụ thể nhé. 
  </t>
   </si>
@@ -73,9 +67,6 @@
     <t>Hiến tạng</t>
   </si>
   <si>
-    <t>Mình muốn hiến tạng/hiến xác cho y học thì đăng ký như thế nào ạ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn, Bạn vui lòng liên hệ Bộ môn Giải phẫu học (trong giờ hành chính): 028 3950 9943 để được hướng dẫn nhé! </t>
   </si>
   <si>
@@ -83,9 +74,6 @@
   </si>
   <si>
     <t>Trung tâm U Máu cơ sở 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bé nhỏ muốn điều trị u máu? </t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn, bạn có thể đưa bé đến Trung tâm U máu tại cơ sở 3 của Bệnh viện Đại học Y Dược TPHCM. Trung tâm U máu khám và điều trị các trường hợp u máu nhũ nhi, dị dạng tĩnh mạch, giãn mạch, sẹo, bớt rượu vang, bớt Ota, bớt bẩm sinh, bớt cafe sữa và các dạng bớt khác, đốm nâu, tàn nhang... Sau khi thăm khám, BS sẽ đánh giá tình trạng và tư vấn cụ thể phương pháp điều trị bạn nhé. 
@@ -113,34 +101,22 @@
     <t>Mua Siêu âm atlas</t>
   </si>
   <si>
-    <t>Mình muốn mua cuốn Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương thì mua ở đâu ạ?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Bạn vui lòng liên hệ thư ký khoa Chẩn đoán hình ảnh theo số: 0983 703 587 (trong giờ hành chính) nhé. </t>
   </si>
   <si>
     <t>Hướng dẫn sử dụng thuốc</t>
   </si>
   <si>
-    <t>Con mình đi khám về và đưa đơn thuốc, mình muốn cho con uống nhưng không hiểu rõ đơn cần gặp Bác sĩ hỏi phải làm sao?</t>
-  </si>
-  <si>
     <t>Bạn vui lòng liên hệ Bộ phận tư vấn sử dụng thuốc tại: 028 3952 5295 (trong giờ hành chính) để được hướng dẫn nhé.</t>
   </si>
   <si>
     <t>CMEs</t>
   </si>
   <si>
-    <t>Mình muốn đăng ký học lớp căng chỉ thì phải làm sao? Bệnh viện có nhận đăng ký thực hành 18 tháng không?</t>
-  </si>
-  <si>
     <t>Bạn vui lòng xem các lớp tại: https://khdt.edu.vn/</t>
   </si>
   <si>
     <t>Quy trình khám chữa bệnh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quy trình đặt hẹn khám bệnh như thế nào? </t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn, để tránh chờ đợi lâu, bạn vui lòng đặt lịch khám bệnh trực tuyến qua tổng đài 1900 2115 hoặc tải ứng dụng: UMC- Care (App Store, Google Play), xem hướng dẫn tại: https://www.bvdaihoc.com.vn/upload/images/cms/2023/10/11/UMC%20Care%20a4%20-%20adapt.pdf 
@@ -217,32 +193,20 @@
     <t>Cắt thắng lưỡi cho bé</t>
   </si>
   <si>
-    <t xml:space="preserve">Bé muốn cắt thắng lưỡi? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn, 
 Bệnh viện có cắt thắng lưỡi cho bé dưới 3 tháng bạn nhé. Thông tin chi tiết, vui lòng liên hệ phòng khám Nhi (trong giờ hành chính) theo số điện thoại 028 3952 5144. </t>
   </si>
   <si>
-    <t xml:space="preserve"> Khám hậu Covid khám phòng khám nào? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Bạn có thể đăng ký khám các chuyên khoa tương ứng với triệu chứng của mình. Bạn vui lòng cho biết triệu chứng để Bệnh viện tư vấn chuyên khoa phù hợp với bạn nhé </t>
   </si>
   <si>
     <t>Mắt lé</t>
   </si>
   <si>
-    <t xml:space="preserve">Bệnh viện Đại học Y Dược TPHCM có điều trị mắt lé không? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Bệnh viện có điều trị mắt lé bạn nhé. Bạn vui lòng đến khám để được Bác sĩ thăm khám và tư vấn cụ thể. Bạn chọn khám tại Phòng khám Mắt - ThS BS. Ngô Nguyễn Thu Hằng nhé. </t>
   </si>
   <si>
     <t>HIV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bệnh viện có xét nghiệm HIV không? </t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn. Bệnh viện có thực hiện xét nghiệm này, bạn đến khu B quầy Bác sĩ tư vấn để được BS cho chỉ định thực hiện và tư vấn về chi phí nhé. 
@@ -252,55 +216,34 @@
     <t>Dị ứng</t>
   </si>
   <si>
-    <t xml:space="preserve">Xét nghiệm tìm ra dị ứng  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bạn vui lòng đặt khám tại Phòng khám Dị ứng - Miễn dịch lâm sàng. Bác sĩ cho bạn chỉ định xét nghiệm nhé. </t>
   </si>
   <si>
-    <t xml:space="preserve">Truớc khi nội sôi dạ dày cần nhịn ăn bao lâu ạ </t>
-  </si>
-  <si>
     <t>Bạn vui lòng nhịn ăn từ 8-10 tiếng nhé.</t>
   </si>
   <si>
     <t>Toa thuốc</t>
   </si>
   <si>
-    <t>Tôi không tái khám được, có thể nhờ người thân mua thuốc theo toa thuốc cũ không?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Người bệnh không nên uống lại toa thuốc cũ nếu như không có chỉ định của Bác sĩ, bạn vui lòng tái khám để Bác sĩ cho chỉ định phù hợp nhé. </t>
   </si>
   <si>
     <t>Thay toa thuốc phù hợp cơ địa</t>
   </si>
   <si>
-    <t>Mình uống thuốc đơn Bác sĩ kê bị chóng mặt và mệt. Cho hỏi có thể thay bằng thuốc gì?</t>
-  </si>
-  <si>
     <t>Chào bạn. Vui lòng đặt tái khám để Bác sĩ thăm khám tình trạng và kê lại đơn phù hợp ạ. Để tránh thời gian chờ đợi, bạn vui lòng đặt lịch khám bệnh trực tuyến qua tổng đài 1900 2115 hoặc tải ứng dụng: UMC Care (App Store, Google Play). Xem hướng dẫn tại: https://www.bvdaihoc.com.vn/upload/images/cms/2023/10/11/UMC%20Care%20a4%20-%20adapt.pdf</t>
   </si>
   <si>
     <t>Điều trị nội trú</t>
   </si>
   <si>
-    <t>Mình muốn nhập viện mổ thay khớp thì làm sao?</t>
-  </si>
-  <si>
     <t>Chào bạn. Bạn vui lòng đặt khám, Bác sĩ sẽ cho bạn chỉ định nhập viện và hướng dẫn quy trình cụ thể. Để tránh thời gian chờ đợi, bạn vui lòng đặt lịch khám bệnh trực tuyến qua tổng đài 1900 2115 hoặc tải ứng dụng: UMC Care (App Store, Google Play). Xem hướng dẫn tại: https://www.bvdaihoc.com.vn/upload/images/cms/2023/10/11/UMC%20Care%20a4%20-%20adapt.pdf</t>
   </si>
   <si>
-    <t>Xem thông tin bệnh</t>
-  </si>
-  <si>
     <t>Chào bạn: vu lòng xem thông tin về các loại bệnh tại: https://www.bvdaihoc.com.vn/Home/ViewDetail/3163#maincontent</t>
   </si>
   <si>
     <t>Tư vấn gói sinh</t>
-  </si>
-  <si>
-    <t>Bệnh viện có những gói sinh nào?</t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn, 
@@ -349,9 +292,6 @@
     <t>Tư vấn dịch vụ sinh</t>
   </si>
   <si>
-    <t>Mình có nhu cầu sính mổ chủ động BV có thể tư vấn dùm mình</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn, vui lòng liên hệ Khoa Phụ sản Bệnh viện Đại học Y Dược TPHCM (028) 3952 5230 (trong giờ hành chính) 
 Thân chào bạn. </t>
   </si>
@@ -359,25 +299,16 @@
     <t>Dịch vụ phá thai</t>
   </si>
   <si>
-    <t>Cho hỏi Bệnh viện có phá thai không?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn, hiện tại Bệnh viện chưa triển khai dịch vụ này nhé. Nếu bạn cần hỗ trợ các vấn đề khác, Bệnh viện sẵn lòng tư vấn cho bạn. </t>
   </si>
   <si>
     <t xml:space="preserve">Mua sổ tay Can thiệp chăm sóc điều dưỡng </t>
   </si>
   <si>
-    <t>Mình muốn mua cuốn Can thiệp chăm sóc điều dưỡng của BV</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn. Bạn vui lòng liên hệ Phòng Điều dưỡng BV ĐHYD TPHCM theo điện thoại 028 3952 5377 (trong giờ hành chính) để được hướng dẫn cụ thể nhé. </t>
   </si>
   <si>
     <t>Khám tại Phòng khám Quốc tế</t>
-  </si>
-  <si>
-    <t>BV cho mình hỏi có khám dịch vụ không?</t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn, Bệnh viện không có khám dịch vụ. Tuy nhiên, bạn có thể đăng ký khám tại phòng khám quốc tế dành cho khách hàng trong và ngoài nước. Việc tư vấn, khám bệnh, chẩn đoán, xét nghiệm ban đầu được thực hiện ngay tại phòng khám, giúp người bệnh rút ngắn thời gian chờ đợi, di chuyển và thực hiện cận lâm sàng. Người bệnh được nhân viên y tế hỗ trợ ở tất cả các khâu khám chữa bệnh: đăng ký khám bệnh, khám bệnh, thực hiện cận lâm sàng và mua thuốc. Khu vực chờ riêng tư, tiện nghi, wifi miễn phí và có hỗ trợ phiên dịch tiếng Anh, Hoa, Hàn Quốc, Campuchia,…  
@@ -387,9 +318,6 @@
     <t>Hoàn tiền dịch vụ cận lâm sàng, và các dịch vụ đặt khám</t>
   </si>
   <si>
-    <t>Cho hỏi mình cọc tiền nội soi rồi giờ không muốn nữa có hoàn tiền lại không ạ?</t>
-  </si>
-  <si>
     <t>Chào bạn. Vui lòng liên hệ phòng Tài chính Kế toán - bộ phận Hoàn tiền tại: 028 3952 5269 (trong giờ hành chính). Thân chào bạn.</t>
   </si>
   <si>
@@ -402,25 +330,16 @@
     <t>Phát hành hóa đơn</t>
   </si>
   <si>
-    <t>Mình muốn xin hóa đơn để nộp cho bảo hiểm, nhưng tới giờ chưa nhận được thì làm sao?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn, Bạn vui lòng liên hệ bộ phận phát hành hoá đơn ngoại trú (trong giờ hành chính) theo số điện thoại sau 028 3952 5269 nhé. </t>
   </si>
   <si>
     <t>Tra cứu hóa đơn</t>
   </si>
   <si>
-    <t>Muốn tra cứu hóa đơn thì vào đâu?</t>
-  </si>
-  <si>
     <t>Bạn vui lòng truy cập: https://hoadon.umc.edu.vn/ (Xem hướng dẫn tại: https://hoadon.umc.edu.vn/tim-hieu-hoa-don/Huong-dan-tra-cuu-hoa-don/14)</t>
   </si>
   <si>
     <t>Lịch khám của Bệnh viện</t>
-  </si>
-  <si>
-    <t>Cho mình hỏi Bệnh viện có khám ngoài giờ, hay Thứ 7, Chủ Nhật không?</t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn. Bệnh viện làm việc theo khung giờ như sau và không khám ngoài giờ nhé: 
@@ -433,17 +352,11 @@
     <t>Giao thuốc tại nhà</t>
   </si>
   <si>
-    <t>Bệnh viện có dịch vụ giao thuốc tại nhà không? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Chào bạn,  
 Hiện tại, Bệnh viện chưa triển khai dịch vụ bán thuốc online và giao thuốc tận nhà. Nếu trước đó người bệnh đã khám tại Bệnh viện, bạn vui lòng cung cấp tên Phòng khám để Bệnh viện cung cấp số điện thoại tư vấn nhé! </t>
   </si>
   <si>
     <t>Khám online</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bệnh viện có dịch vụ khám bệnh trực tuyến hay tại nhà không? </t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn,  
@@ -452,9 +365,6 @@
   </si>
   <si>
     <t>Giờ thăm bệnh</t>
-  </si>
-  <si>
-    <t>Giờ thăm bệnh khoa Chấn thương chỉnh hình từ mấy giờ?</t>
   </si>
   <si>
     <t xml:space="preserve">Chào bạn, mỗi khoa trong Bệnh viện có thời gian thăm bệnh khác nhau, cụ thể vui lòng xem tại: https://umceduvn-my.sharepoint.com/:i:/g/personal/data3_truyenthong_umc_edu_vn/EaNKJVARG8FMr_OkBByybT4B6IQR3CgOW9kXyJH34agzgA?e=aolgzb
@@ -494,9 +404,6 @@
     <t>Cơ sở vật chất</t>
   </si>
   <si>
-    <t>Mình muốn xem các loại giường thì xem ở đâu?</t>
-  </si>
-  <si>
     <t>Bạn vui lòng truy câp: https://www.bvdaihoc.com.vn/Home/ViewDetail/7#maincontent</t>
   </si>
   <si>
@@ -526,9 +433,6 @@
     <t>Cộng đồng người bệnh</t>
   </si>
   <si>
-    <t>Bệnh viện có các cộng đồng người bệnh nào?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Bệnh viện có nhóm Zalo cộng đồng người bệnh, để tham gia, vui lòng truy cập 
 Cộng đồng người bệnh Parkinson: https://zalo.me/g/iaqnmo163 
 Cộng đồng người bệnh Đái tháo đường: https://zalo.me/g/adrawr283 
@@ -610,44 +514,139 @@
     <t>Chuyển hướng khám tổng quát hoặc theo triệu chứng do phòng khám hậu COVID đã ngưng hoạt động</t>
   </si>
   <si>
-    <t>Tôi muốn biết chi phí khám chuyên khoa tại Bệnh viện là bao nhiêu?</t>
-  </si>
-  <si>
-    <t>Tôi muốn biết chi phí các loại khám tổng quát tại Bệnh viện là bao nhiêu?</t>
-  </si>
-  <si>
-    <t>Bạn cho biết chi phí tiêm vaccine HPV là bao nhiêu?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Xin cho tôi biết chi tiết về bảng giá tiêm chủng tại bệnh viện này?
-</t>
-  </si>
-  <si>
-    <t>Bệnh viện có bao nhiêu cơ sở?</t>
-  </si>
-  <si>
-    <t>Xin cho tôi biết chi tiết về bảng giá tiêm chủng tại bệnh viện này?</t>
-  </si>
-  <si>
-    <t>Làm thế nào để tham gia các chương trình trực tiếp, hội thảo nhận quà và nghỉ phép?</t>
-  </si>
-  <si>
-    <t>Làm thế nào để đăng ký khám tại phòng khám Ung bướu của Bệnh viện và đặt lịch trực tuyến?</t>
-  </si>
-  <si>
-    <t>Làm thế nào để liên hệ và sử dụng dịch vụ vận chuyển cấp cứu của Bệnh viện Đại học Y Dược TPHCM?</t>
-  </si>
-  <si>
-    <t>Lịch khám của Bệnh viện và Bác sĩ?</t>
-  </si>
-  <si>
-    <t>Đăng ký khám bệnh?</t>
-  </si>
-  <si>
-    <t>Xem thông tin sức khỏe hữu ích?</t>
-  </si>
-  <si>
-    <t>Làm thế nào để đổi lịch khám và nhận hoàn tiền tại Bệnh viện?</t>
+    <t>Tôi muốn hỏi về Bảo hiểm Y tế tại Bệnh viện?; cho em xin thông tin về bảo hiểm y tế được không ạ?; bảo hiểm y tế có xài được cho bệnh viện này ko ?; bảo hiểm y tế chi trả những dịch vụ nào ở bệnh viện?; mức chi trả của bảo hiểm y tế tại đây là bao nhiêu?; thủ tục sử dụng bảo hiểm y tế tại bệnh viện như thế nào?; tôi cần mang theo những giấy tờ gì khi sử dụng bảo hiểm y tế?; tôi có thể sử dụng thẻ bảo hiểm y tế của tỉnh khác tại đây không?; bệnh viện có áp dụng bảo hiểm y tế trái tuyến không?; nếu tôi quên mang thẻ bảo hiểm y tế thì sao?; tôi có thể đăng ký khám bảo hiểm y tế ban đầu tại đây không?; bệnh viện có hỗ trợ làm thủ tục cấp lại thẻ bảo hiểm y tế không?; tôi có thể mua bảo hiểm y tế ở đâu?; bảo hiểm y tế có bao gồm những loại khám nào?; tôi có thể tìm hiểu thêm thông tin về bảo hiểm y tế ở đâu?; tôi cần liên hệ với ai để được giải đáp thắc mắc về bảo hiểm y tế?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có chấp nhận bảo hiểm y tế ngoài tỉnh không?; Bệnh viện có tiếp nhận bệnh nhân sử dụng bảo hiểm y tế trái tuyến không?; Bệnh viện có nhận khám bệnh cho người có bảo hiểm y tế không cùng tuyến không?; Tôi có thể sử dụng bảo hiểm y tế của tỉnh khác tại bệnh viện này được không?; Mức hưởng bảo hiểm y tế trái tuyến tại bệnh viện là bao nhiêu?; Thủ tục khám chữa bệnh bảo hiểm y tế trái tuyến như thế nào?; Tôi cần mang theo giấy tờ gì khi khám bảo hiểm y tế trái tuyến?; Bệnh viện có yêu cầu giấy chuyển viện khi khám bảo hiểm y tế trái tuyến không?; Tôi có thể đăng ký khám bảo hiểm y tế ban đầu tại bệnh viện này dù không cùng tuyến được không?; Bệnh viện có hỗ trợ làm thủ tục chuyển tuyến bảo hiểm y tế không?; Nếu tôi khám bảo hiểm y tế trái tuyến, tôi có phải trả thêm chi phí nào không?; Tôi có thể tìm hiểu thêm thông tin về bảo hiểm y tế trái tuyến ở đâu?; Tôi nên liên hệ với ai để được giải đáp thắc mắc về bảo hiểm y tế trái tuyến tại bệnh viện?</t>
+  </si>
+  <si>
+    <t>Tôi muốn đăng ký hiến tạng/hiến xác cho y học thì làm như thế nào?; Thủ tục đăng ký hiến tạng/hiến xác cho y học là gì?; Cách đăng ký hiến tạng/hiến xác cho y học như thế nào?; Tôi có thể đăng ký hiến tạng/hiến xác ở đâu?; Điều kiện để đăng ký hiến tạng/hiến xác là gì?; Độ tuổi nào có thể đăng ký hiến tạng/hiến xác?; Tôi cần chuẩn bị những giấy tờ gì để đăng ký hiến tạng/hiến xác?; Gia đình tôi có cần đồng ý khi tôi đăng ký hiến tạng/hiến xác không?; Sau khi đăng ký hiến tạng/hiến xác, tôi có cần làm gì nữa không?; Tôi có thể hủy đăng ký hiến tạng/hiến xác không?; Hiến tạng/hiến xác có vi phạm pháp luật không?; Hiến tạng/hiến xác có ảnh hưởng đến tang lễ không?; Tôi có thể tìm hiểu thêm thông tin về hiến tạng/hiến xác ở đâu?; Tôi có thể liên hệ với ai để được tư vấn về hiến tạng/hiến xác?; Hiến tạng/hiến xác có ý nghĩa như thế nào?; Có những câu chuyện cảm động nào về hiến tạng/hiến xác không?</t>
+  </si>
+  <si>
+    <t>Con tôi bị u máu, muốn điều trị thì phải làm sao?; Trẻ em bị u máu cần điều trị như thế nào?; Làm thế nào để điều trị u máu cho trẻ em?; U máu ở trẻ em có nguy hiểm không?; Bệnh viện có chuyên khoa điều trị u máu cho trẻ em không?; Bác sĩ nào chuyên điều trị u máu ở trẻ em tại bệnh viện?; Các phương pháp điều trị u máu ở trẻ em là gì?; Chi phí điều trị u máu cho trẻ em là bao nhiêu?; Bảo hiểm y tế có chi trả cho việc điều trị u máu không?; Tôi cần chuẩn bị gì khi đưa con đi khám u máu?; Tôi có thể đặt lịch khám cho con trực tuyến không?; Sau khi điều trị u máu, trẻ cần được chăm sóc như thế nào?; U máu có thể tái phát không?; Tôi có thể tìm hiểu thêm thông tin về u máu ở trẻ em ở đâu?; Bệnh viện có chương trình hỗ trợ điều trị u máu cho trẻ em không?</t>
+  </si>
+  <si>
+    <t>Gọi xe cấp cứu?; Liên hệ với đội cấp cứu?; Yêu cầu hỗ trợ y tế khẩn cấp?; Gọi người cứu hộ?; Gọi dịch vụ cấp cứu y tế?; Cần xe cứu thương gấp?; Gọi 115 ngay lập tức?; Tôi cần hỗ trợ y tế khẩn cấp?; Có người bị thương nặng, cần xe cấp cứu?; Cần gọi cấp cứu?; Xin hãy giúp đỡ, cần xe cấp cứu?; Gọi bác sĩ nhanh lên?; Có trường hợp khẩn cấp, cần xe cấp cứu?; Cần sự trợ giúp của y tế ngay lập tức?; Có người cần được sơ cứu?; Tình hình nguy kịch, cần xe cấp cứu?; Gọi đội cứu hộ y tế?; Cần xe cấp cứu đến ngay?; Xin hãy đến giúp đỡ, có người bị nạn?</t>
+  </si>
+  <si>
+    <t>Tôi muốn mua sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương, mua ở đâu?; Làm sao để mua cuốn Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương?; Mua sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương ở đâu?; Sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương có bán tại bệnh viện không?; Tôi có thể đặt mua sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương online không?; Giá sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương là bao nhiêu?; Sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương có phiên bản tiếng Anh không?; Tôi có thể tìm mua sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương ở hiệu sách nào?; Ngoài sách Siêu âm Atlas, Thầy Nguyễn Quang Thái Dương còn có những cuốn sách nào khác?; Làm thế nào để liên hệ với nhà xuất bản sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương?; Sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương có được giảm giá không?; Tôi có thể mua sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương cũ không?; Sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương có ebook không?; Tôi có thể đọc thử sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương ở đâu?; Ai nên đọc sách Siêu âm Atlas của Thầy Nguyễn Quang Thái Dương?</t>
+  </si>
+  <si>
+    <t>Tôi không hiểu đơn thuốc của con sau khi đi khám, cần gặp bác sĩ hỏi thế nào?; Làm sao để hỏi bác sĩ về đơn thuốc của con tôi?; Đơn thuốc của con tôi không rõ ràng, cần gặp bác sĩ hỏi như thế nào?; Tôi có thể liên hệ với bác sĩ đã khám cho con tôi để hỏi về đơn thuốc bằng cách nào?; Tôi muốn giải thích rõ hơn về đơn thuốc của con, tôi có thể gặp lại bác sĩ được không?; Tôi có thể đặt lịch hẹn với bác sĩ để hỏi về đơn thuốc của con không?; Bệnh viện có dịch vụ tư vấn về đơn thuốc không?; Tôi có thể gửi ảnh đơn thuốc cho bác sĩ để hỏi không?; Nếu tôi không thể đến bệnh viện, tôi có thể hỏi về đơn thuốc qua điện thoại hoặc email không?; Tôi cần mang theo những gì khi đến gặp bác sĩ để hỏi về đơn thuốc?; Bệnh viện có cung cấp dịch vụ phiên dịch đơn thuốc không?; Chi phí cho việc tư vấn về đơn thuốc là bao nhiêu?; Tôi có thể yêu cầu bác sĩ viết lại đơn thuốc rõ ràng hơn không?; Ngoài bác sĩ, tôi có thể hỏi ai về đơn thuốc của con?; Tôi nên làm gì nếu tôi nghi ngờ đơn thuốc của con bị sai?</t>
+  </si>
+  <si>
+    <t>Mình muốn đăng ký học lớp căng chỉ thì phải làm sao?; Bệnh viện có nhận đăng ký thực hành 18 tháng không?; Bệnh viện có tổ chức lớp học căng chỉ không?; Lịch khai giảng lớp căng chỉ tiếp theo là khi nào?; Học phí của lớp căng chỉ là bao nhiêu?; Thời gian học của lớp căng chỉ là bao lâu?; Nội dung của lớp căng chỉ bao gồm những gì?; Ai có thể tham gia lớp căng chỉ?; Điều kiện để đăng ký học lớp căng chỉ là gì?; Tôi cần chuẩn bị những gì để đăng ký học lớp căng chỉ?; Tôi có thể đăng ký học lớp căng chỉ trực tuyến không?; Bệnh viện có cấp chứng chỉ sau khi hoàn thành khóa học căng chỉ không?; Có hỗ trợ việc làm sau khi học xong lớp căng chỉ không?; Tôi có thể tìm hiểu thêm thông tin về lớp căng chỉ ở đâu?; Tôi có thể liên hệ với ai để được tư vấn về lớp căng chỉ?</t>
+  </si>
+  <si>
+    <t>Cách đặt hẹn khám bệnh tại bệnh viện như thế nào?; Thủ tục đặt hẹn khám bệnh ra sao?; Làm sao để đặt hẹn khám bệnh?; Tôi có thể đặt hẹn khám bệnh qua điện thoại không?; Tôi có thể đặt hẹn khám bệnh trực tuyến không?; Tôi có thể đặt hẹn khám bệnh qua ứng dụng di động không?; Tôi cần cung cấp những thông tin gì khi đặt hẹn khám bệnh?; Tôi có thể đặt hẹn khám bệnh cho người khác không?; Tôi có thể chọn bác sĩ khi đặt hẹn khám bệnh không?; Tôi có thể chọn ngày giờ khám bệnh khi đặt hẹn không?; Tôi có thể thay đổi lịch hẹn khám bệnh không?; Tôi cần làm gì nếu tôi đến trễ giờ hẹn khám bệnh?; Tôi có thể hủy lịch hẹn khám bệnh không?; Nếu tôi hủy lịch hẹn khám bệnh, tôi có được hoàn tiền không?; Tôi có thể đặt hẹn khám bệnh vào cuối tuần hoặc ngày lễ không?; Tôi có thể đặt hẹn khám bệnh cho nhiều người cùng lúc không?; Tôi có thể đặt hẹn khám bệnh cho nhiều chuyên khoa khác nhau không?; Tôi có thể yêu cầu dịch vụ khám bệnh tại nhà không?; Tôi có thể tìm hiểu thêm thông tin về đặt hẹn khám bệnh ở đâu?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tôi muốn biết chi phí khám chuyên khoa của Bệnh viện?; Tôi muốn hỏi về chi phí khám chuyên khoa tại Bệnh viện?; Tôi muốn tìm hiểu về giá khám chuyên khoa ở Bệnh viện?; Xin cho tôi biết chi phí khám chuyên khoa của Bệnh viện?; Tôi muốn biết giá dịch vụ khám chuyên khoa ở Bệnh viện?; Tôi cần biết chi phí để khám chuyên khoa tại Bệnh viện?; Làm ơn cho tôi thông tin về giá khám chuyên khoa tại Bệnh viện?; Tôi cần tìm hiểu chi phí khám chuyên khoa của Bệnh viện?; Chi phí khám chuyên khoa tại Bệnh viện là bao nhiêu?; Giá khám chuyên khoa ở Bệnh viện như thế nào?; Tôi muốn biết chi phí khám chuyên khoa ở Bệnh viện là bao nhiêu? </t>
+  </si>
+  <si>
+    <t>Tôi muốn biết chi phí các loại khám tổng quát tại Bệnh viện là bao nhiêu?; Xin cho tôi biết giá khám tổng quát tại Bệnh viện?; Tôi cần thông tin về chi phí các hình thức khám tổng quát ở Bệnh viện?; Cho tôi hỏi về các loại khám tổng quát và chi phí tại Bệnh viện?; Tôi muốn biết giá các dịch vụ khám tổng quát ở Bệnh viện?; Các hình thức khám tổng quát tại Bệnh viện có mức chi phí như thế nào?; Tôi cần biết giá các dịch vụ khám tổng quát của Bệnh viện?; Xin thông tin về chi phí khám tổng quát ở Bệnh viện?; Tôi muốn tìm hiểu chi phí khám tổng quát tại Bệnh viện là bao nhiêu?; Các loại khám tổng quát ở Bệnh viện có chi phí ra sao?; Bệnh viện có các gói khám tổng quát nào?; Gói khám tổng quát cơ bản bao gồm những gì?; Gói khám tổng quát nâng cao bao gồm những gì?; Chi phí khám tổng quát có bao gồm chi phí xét nghiệm không?; Chi phí khám tổng quát có bao gồm chi phí siêu âm không?; Tôi có thể sử dụng bảo hiểm y tế để thanh toán chi phí khám tổng quát không?; Có chương trình giảm giá nào cho khám tổng quát không?; Tôi có thể đặt lịch khám tổng quát trực tuyến không?; Tôi cần chuẩn bị gì trước khi đi khám tổng quát?; Kết quả khám tổng quát có được gửi về nhà không?</t>
+  </si>
+  <si>
+    <t>Xin thông tin về giá tiêm vaccine HPV?; Tôi cần tìm hiểu về chi phí tiêm HPV?; Cho tôi biết giá tiêm vaccine HPV là bao nhiêu tiền?; Xin hỏi chi phí tiêm vaccine HPV ở đây là bao nhiêu?; Giá tiêm phòng HPV là bao nhiêu?; Chi phí tiêm chủng HPV là bao nhiêu?; Tiêm ngừa HPV hết bao nhiêu tiền?; Giá vaccine HPV bao nhiêu một mũi?; Bảng giá tiêm HPV như thế nào?; Giá tiêm HPV 9 giá là bao nhiêu?; Giá tiêm HPV 4 giá là bao nhiêu?; Giá tiêm HPV 2 giá là bao nhiêu?; Tiêm HPV có được bảo hiểm y tế chi trả không?; Có chương trình ưu đãi nào khi tiêm HPV không?; Tôi có thể đặt lịch tiêm HPV online được không?; Tôi cần lưu ý gì trước khi tiêm HPV?; Tiêm HPV có tác dụng phụ gì không?; Sau khi tiêm HPV cần kiêng gì?</t>
+  </si>
+  <si>
+    <t>Bảng giá tiêm chủng ở đây như thế nào?; Xin cho tôi biết chi tiết về bảng giá tiêm chủng tại bệnh viện này?; Bảng giá tiêm vaccine ở đây có những mục giá nào?; Tôi muốn xem bảng giá tiêm phòng bệnh ở đây?; Bảng giá tiêm chích ngừa tại phòng khám này là bao nhiêu?; Tôi cần biết bảng giá dịch vụ chăm sóc sức khỏe tiêm ngừa?; Bảng giá tiêm vaccine tại đây có tính phí theo liều hay không?; Bảng giá tiêm ngừa bệnh ở đây có cập nhật mới nhất không?; Xin hỏi bảng giá tiêm bảo vệ ở bệnh viện này?; Bảng giá tiêm vaccine phòng chống bệnh dịch có thay đổi không?; Tôi cần thông tin về danh mục giá tiêm chống dịch tại đây?; Bảng giá chích ngừa vaccine ở đây được áp dụng như thế nào?; Tôi muốn biết bảng giá tiêm vắc-xin tại các trung tâm y tế công cộng?; Xin cho tôi biết danh sách giá tiêm vaccine tại các phòng khám?; Bảng giá tiêm phòng bệnh tại đây có điều chỉnh thường xuyên không?; Tôi cần xem danh sách giá tiêm vaccine mới nhất?; Bảng giá tiêm ngừa bệnh được đăng tải trên website của bệnh viện chưa?; Tôi muốn biết bảng giá chích ngừa vaccine ở các bệnh viện lớn?; Xin cho tôi biết bảng giá tiêm vắc-xin tại các phòng khám tư nhân?; Bảng giá phòng bệnh tiêm vaccine ở đây có sự khác biệt so với các nơi khác không?; Giá tiêm vaccine 5 trong 1 là bao nhiêu?; Giá tiêm vaccine sởi là bao nhiêu?; Giá tiêm vaccine phòng ung thư cổ tử cung là bao nhiêu?; Giá tiêm vaccine cúm mùa là bao nhiêu?; Có chương trình giảm giá nào cho tiêm chủng không?; Tôi có thể thanh toán bằng thẻ bảo hiểm y tế khi tiêm chủng không?; Tôi cần đặt lịch hẹn trước khi đến tiêm chủng không?; Tôi có thể tìm thấy bảng giá tiêm chủng ở đâu?; Tôi có thể được tư vấn về tiêm chủng miễn phí không?</t>
+  </si>
+  <si>
+    <t>Tôi bị loại ung thư nào?; Giai đoạn của ung thư của tôi là gì?; Các triệu chứng của ung thư này là gì?; Ung thư của tôi có di căn chưa?; Ung thư của tôi có thể chữa khỏi được không?; Các phương pháp điều trị ung thư của tôi là gì?; Tác dụng phụ của các phương pháp điều trị ung thư là gì?; Tôi nên chuẩn bị gì cho quá trình điều trị ung thư?; Tôi có thể làm gì để kiểm soát các triệu chứng của ung thư?; Tôi nên thay đổi lối sống như thế nào sau khi được chẩn đoán ung thư?; Tôi có thể tìm kiếm sự hỗ trợ ở đâu?; Tôi có thể tham gia vào các thử nghiệm lâm sàng không?; Tôi có thể làm gì để phòng ngừa ung thư tái phát?; Tôi nên nói chuyện với gia đình và bạn bè về ung thư của mình như thế nào?; Tôi có thể tìm hiểu thêm thông tin về ung thư của mình ở đâu?; Ung thư của tôi ảnh hưởng như thế nào đến tuổi thọ của tôi?; Tôi có thể tiếp tục làm việc trong quá trình điều trị ung thư không?; Tôi có thể du lịch trong quá trình điều trị ung thư không?; Tôi có thể mang thai sau khi điều trị ung thư không?; Tôi có thể hiến tạng sau khi điều trị ung thư không?; Ai có thể giúp tôi đưa ra quyết định về điều trị ung thư?</t>
+  </si>
+  <si>
+    <t>Nội soi là gì?; Tôi cần chuẩn bị gì trước khi thực hiện nội soi?; Quy trình nội soi như thế nào?; Thời gian thực hiện nội soi là bao lâu?; Tôi có thể cảm thấy đau hoặc khó chịu không?; Tác dụng phụ của nội soi là gì?; Sau khi nội soi, tôi cần làm gì để hồi phục?; Nội soi có an toàn không?; Có cần gây mê khi thực hiện nội soi không?; Tôi cần nghỉ ngơi bao lâu sau khi nội soi?; Có những loại nội soi nào tôi có thể thực hiện?; Nội soi có thể phát hiện những bệnh gì?; Sinh thiết qua nội soi là gì?; Có phải làm xét nghiệm nào khác sau nội soi không?; Tôi cần phải nhịn ăn trước khi thực hiện nội soi bao lâu?; Nội soi có thể giúp điều trị bệnh không?; Tôi có thể trở lại công việc ngay sau khi thực hiện nội soi không?; Chi phí thực hiện nội soi là bao nhiêu?; Bảo hiểm có chi trả cho chi phí nội soi không?; Có nguy cơ biến chứng nào liên quan đến nội soi không?; Kết quả nội soi sẽ có sau bao lâu?; Tôi có cần phải thực hiện nội soi định kỳ không?; Có nhóm hỗ trợ nào để tôi có thể tìm hiểu thêm về nội soi không?; Quy trình kiểm tra bên trong cơ thể là gì?; Tôi cần chuẩn bị gì trước khi thực hiện kiểm tra qua ống soi?; Quy trình thực hiện kiểm tra qua ống soi như thế nào?; Thời gian thực hiện kiểm tra qua ống soi là bao lâu?; Tôi có thể cảm thấy đau hoặc khó chịu không trong quá trình kiểm tra qua ống soi?; Tác dụng phụ của kiểm tra qua ống soi là gì?; Sau khi thực hiện kiểm tra qua ống soi, tôi cần làm gì để hồi phục?; Kiểm tra qua ống soi có an toàn không?; Có cần gây mê khi thực hiện kiểm tra qua ống soi không?; Tôi cần nghỉ ngơi bao lâu sau khi thực hiện kiểm tra qua ống soi?; Có những loại kiểm tra qua ống soi nào tôi có thể thực hiện?; Kiểm tra qua ống soi có thể phát hiện những bệnh gì?; Sinh thiết thông qua kiểm tra ống soi là gì?; Có cần làm xét nghiệm nào khác sau kiểm tra qua ống soi không?; Tôi cần phải nhịn ăn trước khi thực hiện kiểm tra qua ống soi bao lâu?; Kiểm tra qua ống soi có thể giúp điều trị bệnh không?; Tôi có thể trở lại công việc ngay sau khi thực hiện kiểm tra qua ống soi không?; Chi phí thực hiện kiểm tra qua ống soi là bao nhiêu?; Bảo hiểm có chi trả cho chi phí kiểm tra qua ống soi không?; Có nguy cơ biến chứng nào liên quan đến kiểm tra qua ống soi không?; Kết quả kiểm tra qua ống soi sẽ có sau bao lâu?; Tôi có cần phải thực hiện kiểm tra qua ống soi định kỳ không?; Có nhóm hỗ trợ nào để tôi có thể tìm hiểu thêm về kiểm tra qua ống soi không?; Phương pháp kiểm tra qua ống soi có phải là lựa chọn tốt nhất cho trường hợp của tôi không?; Có cần phải dùng thuốc trước khi thực hiện kiểm tra qua ống soi không?; Kết quả kiểm tra qua ống soi có được giải thích ngay sau khi thực hiện không?; Tôi có thể ăn uống bình thường sau khi kiểm tra qua ống soi không?; Tôi có cần thực hiện các xét nghiệm khác để xác nhận kết quả của kiểm tra qua ống soi không?; Có phương pháp kiểm tra nào ít xâm lấn hơn không?; Thời gian hồi phục sau kiểm tra qua ống soi có lâu không?; Phương pháp kiểm tra qua ống soi có thể phát hiện các bệnh không liên quan đến tiêu hóa không?; Có cần phải thực hiện nhiều lần kiểm tra qua ống soi không?; Có cần phải thay đổi chế độ ăn uống sau khi thực hiện kiểm tra qua ống soi không?</t>
+  </si>
+  <si>
+    <t>Bé muốn cắt thắng lưỡi?; Bé nhà tôi bị dính thắng lưỡi, cần cắt không?; Cắt thắng lưỡi cho bé ở đâu?; Chi phí cắt thắng lưỡi cho bé là bao nhiêu?; Cắt thắng lưỡi cho bé có đau không?; Cắt thắng lưỡi cho bé có ảnh hưởng gì không?; Độ tuổi nào thì nên cắt thắng lưỡi cho bé?; Quy trình cắt thắng lưỡi cho bé như thế nào?; Sau khi cắt thắng lưỡi cho bé cần lưu ý gì?; Cắt thắng lưỡi cho bé có cần gây mê không?; Bác sĩ nào chuyên cắt thắng lưỡi cho bé ở bệnh viện?; Tôi có thể đặt lịch cắt thắng lưỡi cho bé trực tuyến không?; Bảo hiểm y tế có chi trả cho việc cắt thắng lưỡi không?; Tôi có thể tìm hiểu thêm thông tin về cắt thắng lưỡi cho bé ở đâu?; Cắt thắng lưỡi có giúp bé nói rõ hơn không?</t>
+  </si>
+  <si>
+    <t>Tôi muốn khám hậu Covid thì khám ở đâu?; Khám sau khi bị Covid thì đến khoa nào?; Bị Covid xong muốn đi khám thì đăng ký khám ở đâu?; Bệnh viện có khám cho những người đã khỏi Covid không?; Tôi đã khỏi Covid rồi, giờ muốn kiểm tra sức khỏe thì khám thế nào?; Khám hậu Covid có cần đặt lịch trước không?; Chi phí khám hậu Covid là bao nhiêu?; Các xét nghiệm cần thiết khi khám hậu Covid là gì?; Bệnh viện có gói khám hậu Covid không?; Tôi có thể sử dụng bảo hiểm y tế để khám hậu Covid không?; Triệu chứng hậu Covid thường gặp là gì?; Bệnh viện có điều trị các di chứng hậu Covid không?; Tôi cần lưu ý gì khi khám hậu Covid?; Tôi nên khám hậu Covid sau bao lâu khỏi bệnh?; Tôi có thể tìm hiểu thêm thông tin về khám hậu Covid ở đâu?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có khám mắt lé không?; Bệnh viện mình có chữa lé mắt không?; Ở đây có chữa lác mắt không?; BV ĐHYD có điều trị lé mắt không ạ?; Cho em hỏi bệnh viện có khoa mắt lé không?; Tôi muốn khám mắt lé thì đến đây có được không?; Bệnh viện có tiếp nhận bệnh nhân bị lé mắt không?; Bác sĩ nào chuyên điều trị lé mắt ở bệnh viện?; Chi phí khám và điều trị lé mắt là bao nhiêu?; Bệnh viện có áp dụng phương pháp phẫu thuật lé mắt không?; Thời gian điều trị lé mắt kéo dài bao lâu?; Có những phương pháp điều trị lé mắt nào?; Lé mắt có thể chữa khỏi hoàn toàn không?; Tôi cần chuẩn bị gì trước khi đến khám lé mắt?; Tôi có thể đặt lịch khám lé mắt trực tuyến không?; Bảo hiểm y tế có chi trả cho việc điều trị lé mắt không?</t>
+  </si>
+  <si>
+    <t>Ở bệnh viện có làm xét nghiệm HIV không?; Tôi muốn kiểm tra HIV thì làm ở đâu?; Bệnh viện có dịch vụ thử máu HIV không?; Muốn tầm soát HIV thì đến khoa nào?; Làm xét nghiệm HIV ở bệnh viện có bảo mật không?; Chi phí xét nghiệm HIV là bao nhiêu?; Tôi cần chuẩn bị gì trước khi xét nghiệm HIV?; Kết quả xét nghiệm HIV khi nào có?; Tôi có thể đặt lịch xét nghiệm HIV trước không?; Xét nghiệm HIV có những phương pháp nào?; Xét nghiệm HIV nhanh có chính xác không?; Nếu tôi có kết quả xét nghiệm HIV dương tính thì sao?; Bệnh viện có tư vấn và điều trị HIV không?; Tôi có thể sử dụng bảo hiểm y tế để chi trả cho xét nghiệm HIV không?; Tôi có thể tìm hiểu thêm thông tin về HIV ở đâu?</t>
+  </si>
+  <si>
+    <t>Làm sao để biết mình bị dị ứng gì?; Tôi muốn xét nghiệm dị ứng thì phải làm sao?; Bệnh viện có làm xét nghiệm dị ứng không?; Tôi muốn kiểm tra xem mình bị dị ứng gì?; Làm thế nào để tìm ra nguyên nhân gây dị ứng?; Xét nghiệm dị ứng có những loại nào?; Chi phí xét nghiệm dị ứng là bao nhiêu?; Tôi cần chuẩn bị gì trước khi xét nghiệm dị ứng?; Quy trình xét nghiệm dị ứng như thế nào?; Khi nào tôi có kết quả xét nghiệm dị ứng?; Kết quả xét nghiệm dị ứng có ý nghĩa gì?; Tôi nên làm gì nếu tôi bị dị ứng?; Bệnh viện có bác sĩ chuyên khoa dị ứng không?; Tôi có thể đặt lịch xét nghiệm dị ứng trực tuyến không?; Tôi có thể sử dụng bảo hiểm y tế để chi trả cho xét nghiệm dị ứng không?</t>
+  </si>
+  <si>
+    <t>Chuẩn bị nội soi dạ dày thì nhịn ăn mấy tiếng?; Trước khi soi dạ dày phải nhịn ăn bao lâu?; Nội soi tiêu hóa thì nhịn ăn uống trong bao lâu?; Cần nhịn ăn bao lâu trước khi nội soi bao tử?; Nhịn ăn bao nhiêu tiếng trước khi nội soi dạ dày là đủ?; Nội soi dạ dày có cần nhịn uống nước không?; Tôi có thể uống thuốc trước khi nội soi dạ dày không?; Nếu tôi ăn uống trước khi nội soi dạ dày thì sao?; Nội soi dạ dày có đau không?; Nội soi dạ dày mất bao lâu?; Tôi cần chuẩn bị gì trước khi nội soi dạ dày?; Sau khi nội soi dạ dày tôi có thể ăn uống bình thường không?; Tôi cần lưu ý gì sau khi nội soi dạ dày?; Khi nào tôi có kết quả nội soi dạ dày?; Nếu tôi có thắc mắc về nội soi dạ dày, tôi nên hỏi ai?</t>
+  </si>
+  <si>
+    <t>Tôi muốn mua thuốc theo toa cũ được không?; Có thể lấy thuốc theo đơn thuốc trước đó không?; Người nhà lấy thuốc thay có được không?; Không đi khám lại có mua được thuốc theo toa cũ không?; Bệnh viện có cho mua thuốc theo toa cũ không?; Đơn thuốc của tôi hết hạn chưa?; Tôi có thể mua thuốc theo toa cũ nếu quá hạn không?; Tôi cần mang gì để mua thuốc theo toa cũ?; Nếu tôi muốn mua thêm thuốc thì phải làm sao?; Tôi có thể mua thuốc theo toa cũ ở bất kỳ hiệu thuốc nào không?; Tôi có cần phải đặt lịch hẹn trước để mua thuốc theo toa cũ không?; Nếu bác sĩ kê đơn thuốc mới, tôi có thể mua cả hai loại thuốc cùng lúc không?; Có giới hạn số lượng thuốc tôi có thể mua theo toa cũ không?; Tôi có thể mua thuốc theo toa cũ nếu đơn thuốc bị mất không?; Nếu tôi có thắc mắc về việc mua thuốc theo toa cũ, tôi nên liên hệ với ai?</t>
+  </si>
+  <si>
+    <t>tôi uống thuốc theo toa của bác sĩ nhưng bị chóng mặt và mệt mỏi. Tôi có thể đổi sang thuốc khác không?; Sau khi dùng thuốc bác sĩ kê, tôi cảm thấy chóng mặt và mệt. Có thuốc nào thay thế không?; tôi bị chóng mặt và mệt mỏi sau khi uống thuốc do bác sĩ kê. Có thể thay thuốc bằng loại khác không?; thuốc bác sĩ kê cho tôi làm tôi bị chóng mặt và mệt. Tôi nên thay bằng thuốc gì?; tôi cảm thấy chóng mặt và mệt khi uống thuốc từ bác sĩ. Có thuốc thay thế nào không?; sau khi dùng thuốc theo toa của bác sĩ, tôi bị chóng mặt và mệt mỏi. Có thể chuyển sang thuốc khác không?; tôi cảm thấy mệt mỏi và chóng mặt khi dùng thuốc bác sĩ kê. Có thể thay thuốc bằng loại khác không?; thuốc bác sĩ kê cho tôi gây chóng mặt và mệt. Có thể thay thuốc bằng loại khác không?; tôi bị chóng mặt và mệt mỏi sau khi uống thuốc theo chỉ định của bác sĩ. Có thuốc thay thế nào không?; uống thuốc bác sĩ kê làm tôi cảm thấy mệt và chóng mặt. Tôi có thể thay bằng thuốc khác không?; sau khi dùng thuốc theo đơn của bác sĩ, tôi bị chóng mặt và mệt mỏi. Có thể thay thế bằng thuốc khác không?; tôi bị mệt mỏi và chóng mặt khi uống thuốc bác sĩ kê. Có thuốc nào khác mà tôi có thể sử dụng không?; thuốc bác sĩ kê cho tôi gây ra chóng mặt và mệt. Tôi có thể đổi thuốc không?; tôi cảm thấy chóng mặt và mệt sau khi dùng thuốc bác sĩ kê. Có thể thay đổi thuốc bằng loại khác không?; sau khi uống thuốc theo toa của bác sĩ, tôi bị chóng mặt và mệt mỏi. Có thể sử dụng thuốc khác thay thế không?; tôi nên báo cáo tác dụng phụ này cho bác sĩ như thế nào?; liệu có những tác dụng phụ khác mà tôi cần lưu ý không?; tôi có nên ngừng uống thuốc ngay lập tức không?; có những lựa chọn điều trị thay thế nào cho tình trạng của tôi không?; tôi có thể làm gì để giảm thiểu tác dụng phụ chóng mặt và mệt mỏi?; khi nào tôi nên quay lại gặp bác sĩ để kiểm tra?; tôi có thể dùng thuốc không kê đơn nào để giảm bớt triệu chứng trong thời gian chờ đợi không?; tôi có cần phải làm thêm xét nghiệm nào để xác định nguyên nhân gây ra tác dụng phụ không?; liệu các loại thuốc khác mà tôi đang dùng có thể tương tác với loại thuốc này không?</t>
+  </si>
+  <si>
+    <t>tôi muốn vào viện để phẫu thuật thay khớp. Tôi cần làm gì?; tôi cần nhập viện để thực hiện phẫu thuật thay khớp. Các bước cần theo là gì?; làm thế nào để tôi nhập viện và thực hiện ca mổ thay khớp?; tôi muốn thực hiện phẫu thuật thay khớp tại bệnh viện. Tôi cần chuẩn bị gì?; tôi muốn vào viện để thay khớp. Quy trình nhập viện và phẫu thuật như thế nào?; tôi cần làm gì để nhập viện và thực hiện phẫu thuật thay khớp?; tôi có ý định vào viện để mổ thay khớp. Tôi phải làm các thủ tục gì?; tôi muốn nhập viện để thay khớp. Các bước cần thực hiện để chuẩn bị cho ca mổ là gì?; tôi muốn phẫu thuật thay khớp tại bệnh viện. Tôi nên bắt đầu từ đâu?; tôi cần vào viện để phẫu thuật thay khớp. Có các bước nào cần thực hiện không?</t>
+  </si>
+  <si>
+    <t>tra cứu thông tin về bệnh?; xem dữ liệu về bệnh lý?; tìm hiểu thông tin về bệnh?; đọc thông tin về bệnh?; xem các chi tiết về bệnh?; khám phá thông tin bệnh lý?; xem thông tin liên quan đến bệnh?; đọc dữ liệu về tình trạng bệnh?; tham khảo thông tin về bệnh?; xem thông tin liên quan đến bệnh lý?; tìm kiếm thông tin bệnh?; nghiên cứu về bệnh?; tìm hiểu về triệu chứng bệnh?; đọc về nguyên nhân gây bệnh?; xem thông tin về cách điều trị bệnh?; tìm hiểu về biến chứng của bệnh?; đọc về cách phòng ngừa bệnh?; xem thông tin về chế độ dinh dưỡng cho người bệnh?; tìm hiểu về các loại thuốc điều trị bệnh?; đọc về kinh nghiệm của người bệnh?; tra cứu thông tin y khoa về bệnh?; tìm hiểu về các nghiên cứu mới nhất về bệnh?; xem thông tin về các chuyên gia điều trị bệnh?; đọc về các phương pháp chẩn đoán bệnh?; tìm hiểu về các yếu tố nguy cơ gây bệnh?; xem thông tin về các bệnh liên quan?; đọc về các bài viết chia sẻ về bệnh?; tìm hiểu về các tổ chức hỗ trợ người bệnh?; xem thông tin về các hội thảo về bệnh?; đọc về các câu hỏi thường gặp về bệnh?</t>
+  </si>
+  <si>
+    <t>bệnh viện cung cấp các gói sinh gì?; các gói dịch vụ sinh tại bệnh viện là gì?; bệnh viện có các lựa chọn gói sinh nào?; bệnh viện có những loại gói sinh nào?; bệnh viện cung cấp những gói dịch vụ sinh nào?; các gói sinh con tại bệnh viện gồm những gì?; bệnh viện có các chương trình gói sinh nào?; những gói sinh mà bệnh viện cung cấp là gì?; bệnh viện có các tùy chọn gói sinh nào?; các gói sinh hiện có tại bệnh viện là gì?; gói sinh thường giá bao nhiêu?; gói sinh mổ giá bao nhiêu?; các gói sinh bao gồm những dịch vụ gì?; có gói sinh trọn gói không?; tôi có thể lựa chọn bác sĩ trong gói sinh không?; gói sinh có bao gồm chi phí phòng nghỉ không?; gói sinh có bao gồm chi phí thuốc men không?; tôi có thể tìm hiểu chi tiết về các gói sinh ở đâu?; tôi có thể đăng ký gói sinh khi nào?; có ưu đãi gì khi đăng ký gói sinh sớm không?</t>
+  </si>
+  <si>
+    <t>tôi muốn thực hiện sinh mổ chủ động, bệnh viện có thể cung cấp tư vấn cho tôi không?; tôi có nhu cầu sinh mổ chủ động, bệnh viện có thể hướng dẫn tôi được không?; tôi cần thông tin về sinh mổ chủ động, bệnh viện có thể tư vấn cho tôi không?; bệnh viện có thể giúp tôi tư vấn về sinh mổ chủ động không?; tôi dự định sinh mổ chủ động, bệnh viện có thể hỗ trợ tư vấn cho tôi không?; tôi có ý định thực hiện sinh mổ chủ động, bệnh viện có thể cung cấp thông tin cho tôi không?; tôi cần tư vấn về việc sinh mổ chủ động, bệnh viện có thể hỗ trợ tôi được không?; bệnh viện có thể hướng dẫn tôi về dịch vụ sinh mổ chủ động không?; tôi muốn biết thêm về sinh mổ chủ động, bệnh viện có thể tư vấn cho tôi không?; tôi có nhu cầu sinh mổ chủ động, bệnh viện có thể cung cấp sự tư vấn cần thiết không?; điều kiện để được sinh mổ chủ động là gì?; chi phí sinh mổ chủ động tại bệnh viện là bao nhiêu?; quy trình sinh mổ chủ động diễn ra như thế nào?; sinh mổ chủ động có những ưu điểm và nhược điểm gì?; những rủi ro có thể xảy ra khi sinh mổ chủ động là gì?; sau khi sinh mổ chủ động cần lưu ý những gì?; tôi cần chuẩn bị gì trước khi sinh mổ chủ động?; bác sĩ nào sẽ thực hiện ca sinh mổ chủ động cho tôi?; tôi có thể lựa chọn ngày giờ sinh mổ chủ động không?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có làm dịch vụ bỏ thai không?; Bệnh viện có thực hiện đình chỉ thai không?; Ở đây có làm thủ thuật hút thai không?; Tôi muốn hỏi về dịch vụ nạo thai?; Bệnh viện mình có tiếp nhận bỏ thai không?; Tôi muốn tìm hiểu về việc đình chỉ thai nghén ở bệnh viện được không?; Bệnh viện có dịch vụ phá thai an toàn không?; Bệnh viện có hỗ trợ phá thai không?; Bệnh viện có thực hiện các ca phá thai không?; Chi phí phá thai tại bệnh viện là bao nhiêu?; Thủ tục phá thai tại bệnh viện như thế nào?; Tôi muốn phá thai thì cần chuẩn bị những gì?; Bệnh viện có tư vấn về các phương pháp phá thai không?; Bệnh viện có hỗ trợ tâm lý sau phá thai không?; Có những rủi ro nào khi phá thai?; Phá thai có ảnh hưởng đến sức khỏe sinh sản sau này không?; Tôi cần lưu ý gì sau khi phá thai?; Bệnh viện có cung cấp dịch vụ kế hoạch hóa gia đình không?</t>
+  </si>
+  <si>
+    <t>Làm sao để mua được sách "Can thiệp chăm sóc điều dưỡng" của bệnh viện?; Bệnh viện có bán sách "Can thiệp chăm sóc điều dưỡng" không?; Tôi muốn tìm mua cuốn "Can thiệp chăm sóc điều dưỡng" của BV?; Tôi muốn hỏi về cách thức mua tài liệu "Can thiệp chăm sóc điều dưỡng"?; Bệnh viện có bán tài liệu hướng dẫn chăm sóc điều dưỡng không?; Cho em hỏi về việc mua sách do bệnh viện phát hành?; Tôi muốn đặt mua cuốn sách "Can thiệp chăm sóc điều dưỡng" thì liên hệ ở đâu?; Làm thế nào để mua cuốn Can thiệp chăm sóc điều dưỡng của Bệnh viện?; Tôi có thể mua sách Can thiệp chăm sóc điều dưỡng của Bệnh viện ở đâu?; Cuốn sách Can thiệp chăm sóc điều dưỡng của Bệnh viện có bán ở đâu?; Sách "Can thiệp chăm sóc điều dưỡng" của bệnh viện giá bao nhiêu?; Tôi có thể mua sách "Can thiệp chăm sóc điều dưỡng" trực tuyến không?; Bệnh viện có giao sách "Can thiệp chăm sóc điều dưỡng" tận nơi không?; Tôi có thể đến trực tiếp bệnh viện để mua sách "Can thiệp chăm sóc điều dưỡng" được không?; Sách "Can thiệp chăm sóc điều dưỡng" có phiên bản điện tử không?; Ngoài sách "Can thiệp chăm sóc điều dưỡng", bệnh viện còn phát hành những ấn phẩm nào khác?; Tôi có thể tìm hiểu thêm thông tin về sách "Can thiệp chăm sóc điều dưỡng" ở đâu?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có khám dịch vụ không?; Bệnh viện có cung cấp dịch vụ khám bệnh không?; Bệnh viện có các dịch vụ khám bệnh nào?; Bệnh viện có các loại hình khám dịch vụ không?; Bệnh viện có dịch vụ khám chữa bệnh không?; Bệnh viện có cung cấp các dịch vụ khám chữa bệnh không?; Bệnh viện có khám dịch vụ theo yêu cầu không?; Bệnh viện có khám ngoài giờ không?; Bệnh viện có dịch vụ khám sức khỏe tổng quát không?; Bệnh viện có khám chuyên khoa nào?; Bệnh viện có khám bảo hiểm y tế không?; Bệnh viện có khám cho người nước ngoài không?; Bệnh viện có dịch vụ khám tại nhà không?; Bệnh viện có gói khám sức khỏe nào?; Bệnh viện có dịch vụ khám và điều trị bệnh gì?</t>
+  </si>
+  <si>
+    <t>Nếu tôi đã đặt cọc tiền nội soi nhưng không muốn làm nữa thì có được hoàn tiền không?; Bệnh viện có hoàn tiền đặt cọc nội soi không nếu tôi hủy?; Tôi đã cọc tiền nội soi, giờ không muốn nữa có thể hoàn lại tiền không?; Nếu tôi đã đặt cọc cho dịch vụ nội soi nhưng không muốn làm nữa, có được hoàn tiền không?; Tôi đã đặt cọc tiền cho nội soi, nếu không muốn làm nữa có thể lấy lại tiền không?; Bệnh viện có hoàn lại tiền đặt cọc cho dịch vụ nội soi không nếu tôi hủy?; Tôi muốn xin hóa đơn nộp cho bảo hiểm nhưng vẫn chưa nhận được, phải làm sao?; Làm thế nào để tôi có thể nhận được hóa đơn nộp bảo hiểm mà chưa nhận được?; Tôi chưa nhận được hóa đơn nộp bảo hiểm, cần phải làm gì?; Tôi cần hóa đơn để nộp bảo hiểm nhưng vẫn chưa thấy, tôi phải làm sao?; Làm cách nào để tôi có thể lấy hóa đơn bảo hiểm y tế?; Tôi muốn xin cấp lại hóa đơn bảo hiểm y tế thì phải làm thế nào?; Tôi đã thanh toán viện phí nhưng chưa nhận được hóa đơn, phải làm sao để lấy lại?; Tôi muốn xin lại hóa đơn viện phí để nộp bảo hiểm thì phải làm gì?; Tôi cần hóa đơn viện phí để nộp bảo hiểm, làm thế nào để tôi có thể nhận được?</t>
+  </si>
+  <si>
+    <t>Tôi có thể đổi ngày khám sau khi đã đặt lịch không?; Quy trình hủy lịch khám như thế nào?; Nếu tôi hủy lịch khám, tôi có được hoàn tiền không?; Thời gian hoàn tiền sau khi hủy lịch khám là bao lâu?; Tôi có thể đặt lại lịch khám mới sau khi hủy lịch cũ không?; Có mất phí khi hủy hoặc đổi lịch khám không?; Tôi có thể đổi lịch khám sang ngày khác trong cùng tuần không?; Tôi cần phải hủy lịch khám bao lâu trước ngày đã đặt?; Làm cách nào để biết lịch khám mới đã được đặt thành công?; Tôi có thể đổi lịch khám trực tuyến hay phải liên hệ trực tiếp?; Tôi muốn dời lịch khám sang một ngày khác thì phải làm sao?; Phí hủy lịch khám là bao nhiêu?; Tôi có thể đổi bác sĩ khám sau khi đã đặt lịch không?; Nếu tôi đến khám trễ thì có được khám không?; Tôi có thể bảo lưu lịch khám để sử dụng sau này không?; Làm thế nào để xác nhận lịch khám của tôi?; Tôi có thể yêu cầu khám ngoài giờ hành chính không?</t>
+  </si>
+  <si>
+    <t>Nếu tôi chưa nhận được hóa đơn để nộp cho bảo hiểm thì phải làm sao?; Làm thế nào để tôi nhận được hóa đơn nộp bảo hiểm mà chưa nhận được?; Tôi cần hóa đơn để nộp bảo hiểm nhưng chưa nhận được, phải làm gì?; Tôi chưa có hóa đơn để nộp bảo hiểm y tế, tôi nên làm thế nào?; Tôi cần làm gì để được cấp lại hóa đơn thanh toán bảo hiểm?; Trường hợp chưa nhận được hóa đơn để hoàn bảo hiểm thì phải làm sao?; Thủ tục xin cấp lại hóa đơn để nộp bảo hiểm như thế nào?; Làm sao để tôi có thể lấy lại hóa đơn đã mất để nộp bảo hiểm?</t>
+  </si>
+  <si>
+    <t>Tôi muốn tra cứu hóa đơn thì phải làm như thế nào?; Làm sao để tra cứu hóa đơn của tôi?; Để tra cứu hóa đơn, tôi nên truy cập ở đâu?; Tôi có thể tra cứu hóa đơn ở đâu?; Cách tra cứu hóa đơn như thế nào?; Làm sao để tôi tìm được thông tin hóa đơn của mình?; Tôi cần làm gì để xem hóa đơn của tôi?; Quy trình tra cứu hóa đơn là gì?; Tôi muốn kiểm tra hóa đơn của mình, làm thế nào?; Xem hóa đơn đã thanh toán ở đâu?; Tìm kiếm hóa đơn điện tử ở đâu?; Tôi muốn xem lại hóa đơn, phải làm sao?; Thông tin hóa đơn của tôi được lưu trữ ở đâu?; Làm cách nào để tôi biết được chi tiết hóa đơn?; Tôi có thể in lại hóa đơn của mình không, và làm như thế nào?</t>
+  </si>
+  <si>
+    <t>Lịch khám của tôi là gì?; Tôi cần đặt lịch khám như thế nào?; Có thể kiểm tra lịch khám của tôi ở đâu?; Tôi có thể thay đổi lịch khám không?; Khi nào thì tôi có thể khám được?; Thời gian chờ đợi để có lịch khám là bao lâu?; Có cần phải hẹn trước khi đến khám không?; Tôi có thể hủy lịch khám đã đặt không?; Có cách nào để xem lịch khám của bác sĩ không?; Lịch khám của bệnh viện có thay đổi không?; Tôi có thể đặt lịch khám qua điện thoại không?; Lịch khám có thể được xác nhận lại không?; Tôi có thể biết lịch khám của các bác sĩ chuyên khoa không?; Có dịch vụ nhắc lịch khám không?; Có thể xem lịch khám online không?; Lịch khám có bao gồm cả ngày cuối tuần không?; Có thể thay đổi thời gian khám sau khi đã đặt không?; Tôi cần mang theo giấy tờ gì khi đến khám theo lịch?; Lịch khám của tôi có bị ảnh hưởng bởi các ngày nghỉ lễ không?</t>
+  </si>
+  <si>
+    <t>Dịch vụ giao thuốc tận nhà có sẵn tại khu vực của tôi không?; Tôi có cần cung cấp thông tin gì thêm để nhận thuốc tại nhà không?; Có phải tôi trả thêm phí cho dịch vụ giao thuốc tận nhà không?; Thời gian giao thuốc tận nhà là bao lâu?; Tôi có thể kiểm tra tình trạng đơn hàng của mình ở đâu?; Có cần ký nhận khi nhận thuốc không?; Nếu tôi không có nhà, thuốc có được để lại ở đâu không?; Dịch vụ giao thuốc tận nhà có hỗ trợ các loại thuốc kê đơn không?; Tôi có thể thay đổi địa chỉ giao thuốc sau khi đã đặt hàng không?; Có thể giao thuốc vào cuối tuần hoặc ngoài giờ làm việc không?; Nếu tôi cần gấp, có thể yêu cầu giao thuốc khẩn cấp không?; Giao thuốc tận nhà có đi kèm với tư vấn y tế không?; Có cần đặt trước bao nhiêu ngày để nhận thuốc tại nhà?; Tôi có thể trả tiền khi nhận thuốc không?; Làm thế nào để biết thuốc đã được giao thành công?; Dịch vụ giao thuốc tận nhà có phục vụ các khu vực nông thôn không?; Có hạn chế gì về loại thuốc có thể giao tận nhà không?; Có chương trình giảm giá hoặc khuyến mãi cho dịch vụ giao thuốc không?; Tôi có thể hủy đơn hàng sau khi đã đặt không?; Nếu thuốc bị hư hỏng trong quá trình giao, tôi nên làm gì?</t>
+  </si>
+  <si>
+    <t>Khám online có được thực hiện qua video call không?; Có cần tải ứng dụng đặc biệt để tham gia khám từ xa không?; Tôi có thể hẹn lịch khám online vào thời gian nào?; Chi phí khám online có khác biệt so với khám trực tiếp không?; Có cần gửi tài liệu hoặc xét nghiệm trước khi khám từ xa không?; Tôi có thể thay đổi hoặc hủy lịch khám online không?; Dịch vụ khám online có hỗ trợ các chuyên khoa khác nhau không?; Khám online có được tư vấn về đơn thuốc và điều trị không?; Tôi có thể nhận kết quả khám online ngay lập tức không?; Có yêu cầu đặc biệt nào về thiết bị hoặc kết nối internet khi khám online không?; Khám online có bảo mật thông tin cá nhân và hồ sơ y tế không?; Tôi có thể liên lạc với bác sĩ sau khi khám online nếu có thêm câu hỏi không?; Dịch vụ khám online có được thực hiện vào cuối tuần không?; Tôi có thể thanh toán phí khám online bằng các phương thức nào?; Khám từ xa có thể điều chỉnh kế hoạch điều trị theo nhu cầu của tôi không?; Có thể thực hiện khám online cho các bệnh lý cấp cứu không?; Khám online có thể bao gồm các dịch vụ xét nghiệm hoặc chẩn đoán không?; Có cần chuẩn bị gì đặc biệt cho buổi khám từ xa không?; Khám online có được hỗ trợ thêm thông tin về thuốc và cách sử dụng không?; Dịch vụ khám online có phù hợp với các bệnh nhân người già không?</t>
+  </si>
+  <si>
+    <t>Giờ thăm bệnh tại bệnh viện là từ mấy giờ đến mấy giờ?; Có giờ thăm bệnh riêng cho các phòng bệnh khác nhau không?; Tôi có thể thăm bệnh nhân vào cuối tuần không?; Có quy định nào về số lượng khách thăm bệnh cùng một lúc không?; Tôi cần đăng ký trước để thăm bệnh nhân không?; Có cần mang theo giấy tờ gì khi đến thăm bệnh nhân không?; Giờ thăm bệnh có thay đổi vào các ngày lễ không?; Tôi có thể thăm bệnh nhân vào buổi tối không?; Có quy định về thời gian thăm bệnh cho trẻ em không?; Có những yêu cầu gì cần tuân thủ trong giờ thăm bệnh?; Nếu tôi không thể thăm bệnh nhân trong giờ quy định, có cách nào để gặp bệnh nhân không?; Có hạn chế gì về số lần thăm bệnh trong một ngày không?; Giờ thăm bệnh có được cập nhật thường xuyên không?; Tôi có thể gọi điện cho bệnh nhân trong giờ thăm bệnh không?; Thời gian thăm bệnh có ảnh hưởng đến giờ điều trị của bệnh nhân không?; Có quy định về trang phục khi đến thăm bệnh nhân không?; Tôi có thể thăm bệnh nhân trong các giờ nghỉ trưa không?; Có những quy định về việc sử dụng thiết bị điện tử trong giờ thăm bệnh không?; Nếu bệnh nhân cần nghỉ ngơi, tôi có thể điều chỉnh giờ thăm không?; Có quy định gì về việc thăm bệnh nhân tại khu vực chăm sóc đặc biệt không?</t>
+  </si>
+  <si>
+    <t>Địa chỉ của bệnh viện là gì?; Làm thế nào để tôi tìm thấy bệnh viện?; Bệnh viện có địa chỉ chính xác nào không?; Có bản đồ chỉ đường đến bệnh viện không?; Bệnh viện có địa chỉ liên hệ khẩn cấp nào không?; Bệnh viện có mấy chi nhánh và địa chỉ của các chi nhánh là gì?; Có điểm đỗ xe gần bệnh viện không?; Địa chỉ của phòng khám thuộc bệnh viện là gì?; Bệnh viện có địa chỉ cụ thể cho các khoa không?; Có dịch vụ vận chuyển hoặc đưa đón bệnh nhân từ bệnh viện không?; Địa chỉ của bệnh viện có dễ tìm không, có chỉ dẫn nào không?; Bệnh viện có thể gửi cho tôi bản đồ đường đến bệnh viện không?; Bệnh viện có thay đổi địa chỉ không?; Tôi có thể tìm thấy thông tin địa chỉ của bệnh viện trên trang web nào?; Bệnh viện có các cơ sở y tế khác không và địa chỉ của chúng là gì?; Có số điện thoại hỗ trợ chỉ đường đến bệnh viện không?; Bệnh viện có địa chỉ gửi thư và bưu phẩm không?; Địa chỉ của các trung tâm chăm sóc đặc biệt trong bệnh viện là gì?; Bệnh viện có bảng chỉ dẫn ngoài trời không?; Địa chỉ của bệnh viện có thay đổi trong các thời gian lễ tết không?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có trang thiết bị y tế hiện đại không?; Các phòng bệnh có được trang bị đầy đủ tiện nghi không?; Phòng mổ có được trang bị thiết bị tiên tiến không?; Bệnh viện có khu vực cấp cứu được trang bị như thế nào?; Có hệ thống điều hòa không khí trong các phòng bệnh không?; Bệnh viện có phòng xét nghiệm được trang bị đầy đủ thiết bị không?; Phòng chăm sóc đặc biệt có các thiết bị hỗ trợ nào?; Có khu vực phục hồi chức năng được trang bị đầy đủ không?; Các khu vực chung như phòng chờ và phòng đón tiếp có được thiết kế tiện nghi không?; Hệ thống thông tin và quản lý bệnh viện có hiện đại không?; Bệnh viện có hệ thống khử khuẩn và tiệt trùng hiệu quả không?; Có khu vực riêng cho việc tiêm chủng và chăm sóc định kỳ không?; Phòng dược có đầy đủ các loại thuốc và thiết bị cần thiết không?; Có hệ thống quản lý chất thải y tế đảm bảo vệ sinh không?; Phòng khám có được trang bị thiết bị chẩn đoán chính xác không?; Có dịch vụ hỗ trợ bệnh nhân về cơ sở vật chất không?; Các phòng bệnh có đầy đủ các tiện nghi cơ bản như nước nóng, internet không?; Bệnh viện có khu vực đón tiếp và hỗ trợ bệnh nhân mới đến như thế nào?; Có các biện pháp đảm bảo an toàn và vệ sinh trong cơ sở vật chất không?; Bệnh viện có các khu vực đặc biệt như phòng y tế cộng đồng không?</t>
+  </si>
+  <si>
+    <t>Tra cứu thông tin y tế hữu ích?; tìm hiểu về kiến thức chăm sóc sức khỏe?; khám phá thông tin y khoa hữu ích?; Tin tức về sức khỏe?; thông tin phòng bệnh?; tìm kiếm dữ liệu y tế cần thiết?; tiếp cận thông tin y tế hữu ích?; tham khảo thông tin y tế hữu ích?</t>
+  </si>
+  <si>
+    <t>đặt lịch khám bệnh?; đăng ký kiểm tra sức khỏe?; ghi danh khám bệnh?; đăng ký thăm khám bệnh?; đặt hẹn khám bệnh?; đăng ký gặp bác sĩ?; đăng ký dịch vụ y tế?; lập lịch khám sức khỏe?; đăng ký tư vấn y tế?; đăng ký chăm sóc y tế?; đặt hẹn kiểm tra sức khỏe?; đăng ký khám sức khỏe định kì?; đăng ký kiểm tra y khoa?; đăng ký dịch vụ khám bệnh?; đăng ký khám bệnh tại bệnh viện?; đăng ký kiểm tra sức khỏe tổng quát?; đăng ký khám và điều trị?; đăng ký dịch vụ kiểm tra sức khỏe định kỳ?</t>
+  </si>
+  <si>
+    <t>thời gian khám bệnh tại Biện viện và với bác sĩ?; Lịch hẹn khám bệnh tại bệnh viện và với bác sĩ?; lịch thăm khám của bệnh viện và bác sĩ?; lịch kiểm tra sức khỏe tại bệnh viện và bác sĩ?; lịch khám bệnh của bệnh viện và bác sĩ?; thời gian khám của bệnh viện và bác sĩ?; lịch khám y tế tại bệnh viện và với bác sĩ?; giờ làm việc của khoa khám bệnh?;lịch trực của bác sĩ?; bệnh viện làm việc từ mấy giờ đến mấy giờ?; có thể đặt lịch khám ngoài giờ không?</t>
+  </si>
+  <si>
+    <t>Bệnh viện có các cộng đồng người bệnh nào?; Bệnh viện có những cộng đồng bệnh nhân nào?; Các nhóm người bệnh tại bệnh viện là gì?; bệnh viện có các cộng đồng bệnh nhân nào?; những cộng đồng người mắc bệnh nào có mặt tại bệnh viện?; bệnh viện cung cấp các cộng đồng bệnh nhân nào?; bệnh viện có những nhóm bệnh nhân nào?; các cộng đồng người bị bệnh tại bệnh viện là gì?; Bệnh viện có câu lạc bộ hỗ trợ bệnh nhân nào?; Bệnh viện có nhóm chia sẻ kinh nghiệm điều trị bệnh nào?; Bệnh viện có tổ chức các buổi gặp mặt cho người bệnh không?; Bệnh viện có cộng đồng hỗ trợ bệnh nhân ung thư không?; Bệnh viện có nhóm hỗ trợ bệnh nhân tiểu đường không?; Bệnh viện có cộng đồng dành cho bệnh nhân tim mạch không?; Bệnh viện có nhóm hỗ trợ bệnh nhân sau phẫu thuật không?; Bệnh viện có các hoạt động dành cho người bệnh và người nhà không?; Bệnh viện có các chương trình tư vấn và hỗ trợ tâm lý cho người bệnh không?</t>
+  </si>
+  <si>
+    <t>xin nghỉ phép?; tham dự sự kiện trực tiếp?; tham gia hội thảo và nhận quà?; nghỉ làm?; tham gia chương trình trực tiếp?; tham gia hội thảo và nhận phần thưởng?; được nghỉ phép?; tham gia sự kiện trực tiếp?; dự hội thảo và nhận quà?; xin nghỉ làm?; tham gia các chương trình trực tiếp?; tham dự hội thảo và nhận quà tặng?; nghỉ việc?; tham gia chương trình trực tiếp?; tham gia hội thảo nhận quà?; nghỉ phép?; tham gia các sự kiện trực tiếp?; dự hội thảo và nhận phần thưởng?; xin nghỉ phép?; tham gia sự kiện trực tiếp?; dự hội thảo và nhận quà?; nghỉ việc?; tham gia chương trình trực tiếp?; tham dự hội thảo và nhận quà?; xin phép nghỉ làm?; tham gia sự kiện livestream?; tham dự hội thảo online và nhận quà?; xin nghỉ không lương?; tham gia buổi phát sóng trực tiếp?; tham gia webinar và nhận quà tặng?; xin nghỉ ốm?; tham gia sự kiện trực tuyến?; tham dự workshop và nhận quà?; xin nghỉ dưỡng sức?; tham gia chương trình phát sóng trực tiếp?; tham gia tọa đàm và nhận phần quà?; xin nghỉ thai sản?; tham gia buổi giao lưu trực tuyến?; tham dự khóa học online và nhận quà?; xin nghỉ hưu?; tham gia chương trình truyền hình trực tiếp?; tham gia hội nghị trực tuyến và nhận quà?</t>
   </si>
 </sst>
 </file>
@@ -762,7 +761,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1047,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="69" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -1074,7 +1073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="1" customFormat="1" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1082,52 +1081,52 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" ht="242.25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" ht="228" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="142.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171" x14ac:dyDescent="0.25">
@@ -1135,83 +1134,83 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="313.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="242.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="C8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="199.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>31</v>
+        <v>123</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="114" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="156.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
@@ -1219,489 +1218,489 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>148</v>
+        <v>125</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>150</v>
+        <v>127</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="99.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="171" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="185.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C19" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D15" s="2" t="s">
+    </row>
+    <row r="20" spans="1:4" ht="171" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D16" s="2" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="171" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="C21" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" ht="171" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>60</v>
+        <v>136</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>63</v>
+        <v>137</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="185.25" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>66</v>
+        <v>138</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="256.5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>68</v>
+        <v>139</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>71</v>
+        <v>140</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>74</v>
+        <v>141</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="171" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="270.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>86</v>
+        <v>145</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="228" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>91</v>
+        <v>147</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="171" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>94</v>
+        <v>148</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="213.75" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="285" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="327.75" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>103</v>
+        <v>151</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="85.5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="356.25" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="313.5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>111</v>
+        <v>154</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="6" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="114" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="228" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="6" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="71.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="299.25" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>122</v>
+        <v>90</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>123</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1727,92 +1726,92 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>124</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>139</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>